<commit_message>
update graphtext and codebook, gitignore
</commit_message>
<xml_diff>
--- a/data_scripts/scripts/Codebook for graphtext update.xlsx
+++ b/data_scripts/scripts/Codebook for graphtext update.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10309"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dwood/Box Sync/sites/ed-data/updated_script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4ACB6AE-3332-2343-8A1D-81748FE6A85F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB0E2218-DB80-9646-AC04-19FCA8BD5B72}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="1840" windowWidth="25600" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="105">
   <si>
     <t>section</t>
   </si>
@@ -165,39 +165,15 @@
     <t>Y</t>
   </si>
   <si>
-    <t>The section number (e.g., 2, 5). This is one of the two numbers that essentially index this document for our own use.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The graph number (e.g., the first multiple of graph 7 would be 71). This is the second index number. </t>
-  </si>
-  <si>
     <t>O</t>
   </si>
   <si>
-    <t>The type of graph this is. Any string is valid - but keep in mind that this looks for keywords "horizontal", "line", and "bar" to make smart decisions.</t>
-  </si>
-  <si>
-    <t>The sources you want on the graph, EXACTLY as you want them  to appear (with the caveat that new lines will not be read)</t>
-  </si>
-  <si>
-    <t>The title of the graph, EXACTLY as you want it to appear (same caveat as above - new lines will not be retained)</t>
-  </si>
-  <si>
-    <t>The notes that you want on the graph, EXACTLY as you want it to appear (same caveat).</t>
-  </si>
-  <si>
-    <t>This is deprecated and you can use it for whatever you would like - as long as EVERY SINGLE MULTIPLE is on its own line</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
     <t>String</t>
   </si>
   <si>
-    <t>Doesn't matter</t>
-  </si>
-  <si>
     <t>Integer</t>
   </si>
   <si>
@@ -208,9 +184,6 @@
   </si>
   <si>
     <t>filename as string</t>
-  </si>
-  <si>
-    <t>This is the name of the csv file you want to read in. Whatever the name of the csv file is, you will get a corresponding json file out. In other words, if for whatever reason, you read data in from the file "theskyisblue.csv", you will get a json in the same folder as your data with the filename "theskyisblue.json"</t>
   </si>
   <si>
     <t>This boolean tells us whether the graph has direct labels (1) or not (0).</t>
@@ -331,19 +304,107 @@
     <t>titleIfSubtitleisMoved</t>
   </si>
   <si>
-    <t xml:space="preserve">The title of the graph, if you plan to have the "title" be more like a "subtitle" in the case of multiple minis. Added by Dan W. </t>
-  </si>
-  <si>
     <t>Any boolean flag that you want to set to true, just type here. Separate all flags with a comma. For example, you can write: "overrideTickCount, hideToolTip" and the top level of the JSON file will include {"overrideTickCount" : true, "hideToolTip" : true}. These will appear in the top level. other examples: connectNull</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>subsection_number</t>
+  </si>
+  <si>
+    <t>The number (1-8) of master section starting with What is College (1) and going to Student Profiles (8)</t>
+  </si>
+  <si>
+    <t>The number (0-N) of the subsection within the master section. Most sections do not have any charts on the homepage (subsection 0), so most sections will not have a subsection 0 in the GraphText file. It does happen later in the site though</t>
+  </si>
+  <si>
+    <t>The number (1-N) of the graph within each subsection. Every mini chart within a Multiples will be numbered individually.</t>
+  </si>
+  <si>
+    <t>The type of graph this is. The options are: bar, bar graph, grouped bar, horizontal bar, horizontal grouped bar, horizontal stacked bar, line, stacked area, stacked bar, table</t>
+  </si>
+  <si>
+    <t>This is the name of the csv file you want to read in. Whatever the name of the csv file is, you will get a corresponding json file out. The name of the csv/json is the concatenation of the section, subsection, and graph number to make 6 digits (adding a leading zero for numbers less than 10). So secction 2, subsection 3, graph 4 would be 020304.csv</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The title of the graph, for when you have multiple mini charts. It is not read into R, but is added into the &lt;Multiples&gt; component in the jsx. We preserve it here for posterity. If this is used, the </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>title</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> section functions like a subtitle. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>The sources you want on the graph, EXACTLY as you want them  to appear. Special characters or formatting (italics, bold, etc) entered in as HTML (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Italic Text</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> must be "&lt;em&gt;Italic Text&lt;/em&gt;"). Ask a dev if you have questions/concerns about this.</t>
+    </r>
+  </si>
+  <si>
+    <t>The title of the graph, EXACTLY as you want it to appear. Special characters or formatting (italics, bold, etc) entered in as HTML (Italic Text must be "&lt;em&gt;Italic Text&lt;/em&gt;"). Ask a dev if you have questions/concerns about this.</t>
+  </si>
+  <si>
+    <t>The notes that you want on the graph, EXACTLY as you want it to appear. Special characters or formatting (italics, bold, etc) entered in as HTML (Italic Text must be "&lt;em&gt;Italic Text&lt;/em&gt;"). Ask a dev if you have questions/concerns about this.</t>
+  </si>
+  <si>
+    <t>This field is a boolean to track whether something is in a multiple. If yes, be sure to enter source, notes, title, subtitles into the jsx.</t>
+  </si>
+  <si>
+    <t>subtitle_for_multiples</t>
+  </si>
+  <si>
+    <t>When you have a multiple that you need to add the subtitle into the jsx file, you can add the subtitle here for posterity, and it will not automatically be added to the chart.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -383,6 +444,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -404,7 +472,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -412,24 +480,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -711,10 +780,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F14" activeCellId="1" sqref="F18 F14"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -726,7 +795,7 @@
     <col min="6" max="6" width="73.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="32">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="32">
       <c r="A1" s="3" t="s">
         <v>37</v>
       </c>
@@ -734,19 +803,19 @@
         <v>40</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="17">
+    <row r="2" spans="1:8" ht="17">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -754,19 +823,19 @@
         <v>42</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>54</v>
+        <v>91</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="17">
+    <row r="3" spans="1:8" ht="17">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -774,19 +843,19 @@
         <v>42</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>54</v>
+        <v>91</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="34">
+    <row r="4" spans="1:8" ht="34">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
@@ -794,333 +863,342 @@
         <v>43</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="34">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="51">
       <c r="A5" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="34">
+      <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="34">
-      <c r="A6" s="5" t="s">
+      <c r="B6" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="85">
+      <c r="A7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="34">
+      <c r="A8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" s="6" t="s">
+      <c r="B8" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="H8" s="10"/>
+    </row>
+    <row r="9" spans="1:8" ht="51">
+      <c r="A9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="H9" s="10"/>
+    </row>
+    <row r="10" spans="1:8" ht="51">
+      <c r="A10" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="H10" s="10"/>
+    </row>
+    <row r="11" spans="1:8" ht="51">
+      <c r="A11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="H11" s="10"/>
+    </row>
+    <row r="12" spans="1:8" ht="51">
+      <c r="A12" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="H12" s="10"/>
+    </row>
+    <row r="13" spans="1:8" ht="34">
+      <c r="A13" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="H13" s="10"/>
+    </row>
+    <row r="14" spans="1:8" ht="17">
+      <c r="A14" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="H14" s="10"/>
+    </row>
+    <row r="15" spans="1:8" ht="17">
+      <c r="A15" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="H15" s="10"/>
+    </row>
+    <row r="16" spans="1:8" ht="34">
+      <c r="A16" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F16" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="34">
-      <c r="A7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="34">
-      <c r="A8" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D8" s="6" t="s">
+      <c r="H16" s="10"/>
+    </row>
+    <row r="17" spans="1:6" ht="34">
+      <c r="A17" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="34">
-      <c r="A9" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="34">
-      <c r="A10" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="34">
-      <c r="A11" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="6" t="s">
+      <c r="D17" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="34">
+      <c r="A18" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D11" s="6" t="s">
+      <c r="C18" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="17">
-      <c r="A12" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="68">
-      <c r="A13" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="17">
-      <c r="A14" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="34">
-      <c r="A15" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="34">
-      <c r="A16" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="17">
-      <c r="A17" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="17">
-      <c r="A18" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>53</v>
-      </c>
       <c r="D18" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="17">
       <c r="A19" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>43</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>80</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="17">
       <c r="A20" s="8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>43</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>71</v>
+        <v>46</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="F20" s="7" t="s">
         <v>72</v>
@@ -1128,402 +1206,442 @@
     </row>
     <row r="21" spans="1:6" ht="17">
       <c r="A21" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>43</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="17">
       <c r="A22" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>43</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="17">
       <c r="A23" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>43</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="17">
       <c r="A24" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>43</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="17">
       <c r="A25" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>43</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="17">
       <c r="A26" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>43</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="17">
       <c r="A27" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="17">
+      <c r="A28" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="17">
+      <c r="A29" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B27" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E27" s="6" t="s">
+      <c r="B29" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F29" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="F27" s="7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="68">
-      <c r="A28" s="8" t="s">
+    </row>
+    <row r="30" spans="1:6" ht="68">
+      <c r="A30" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="F28" s="7" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="34">
-      <c r="A29" s="8" t="s">
+      <c r="B30" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="34">
+      <c r="A31" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="51">
-      <c r="A30" s="8" t="s">
+      <c r="B31" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="51">
+      <c r="A32" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B30" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="F30" s="7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="51">
-      <c r="A31" s="8" t="s">
+      <c r="B32" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="51">
+      <c r="A33" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B31" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="17">
-      <c r="A32" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="F32" s="7" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="17">
-      <c r="A33" s="8" t="s">
-        <v>30</v>
-      </c>
       <c r="B33" s="6" t="s">
         <v>43</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="17">
       <c r="A34" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>43</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="17">
       <c r="A35" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>43</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="17">
       <c r="A36" s="8" t="s">
-        <v>88</v>
+        <v>31</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>43</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="17">
       <c r="A37" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B37" s="6" t="s">
         <v>43</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="17">
       <c r="A38" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="17">
+      <c r="A39" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="17">
+      <c r="A40" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B38" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E38" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="F38" s="7" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="34">
-      <c r="A39" s="8" t="s">
+      <c r="B40" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="34">
+      <c r="A41" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B39" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="F39" s="7" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="119">
-      <c r="A40" s="8" t="s">
+      <c r="B41" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="119">
+      <c r="A42" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B40" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="D40" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E40" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="F40" s="7" t="s">
-        <v>97</v>
+      <c r="B42" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>